<commit_message>
Update of csv file
</commit_message>
<xml_diff>
--- a/Stabla_sve.xlsx
+++ b/Stabla_sve.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="334">
   <si>
     <t xml:space="preserve">ime</t>
   </si>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">porodica</t>
   </si>
   <si>
-    <t xml:space="preserve">list</t>
-  </si>
-  <si>
     <t xml:space="preserve">visina</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t xml:space="preserve">Quercus trojana</t>
   </si>
   <si>
-    <t xml:space="preserve">makedonski_hrast_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 20 m</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t xml:space="preserve">Betula pubescens</t>
   </si>
   <si>
-    <t xml:space="preserve">cretna_breza_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 do 20 m</t>
   </si>
   <si>
@@ -102,7 +93,7 @@
     <t xml:space="preserve">glatka, gruba i ispucana</t>
   </si>
   <si>
-    <t xml:space="preserve">cretna_breza_korsnja.jpg</t>
+    <t xml:space="preserve">cretna_breza_krosnja.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.plantea.com.hr/cretna-breza/</t>
@@ -114,9 +105,6 @@
     <t xml:space="preserve">Acer monspessulanum</t>
   </si>
   <si>
-    <t xml:space="preserve">maklen_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">5 do 15 m</t>
   </si>
   <si>
@@ -141,9 +129,6 @@
     <t xml:space="preserve">Alnus incana</t>
   </si>
   <si>
-    <t xml:space="preserve">bijela_joha_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">bijela_joha_plod.jpg</t>
   </si>
   <si>
@@ -165,9 +150,6 @@
     <t xml:space="preserve">Acer platanoides</t>
   </si>
   <si>
-    <t xml:space="preserve">mlijec_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">mlijec_plod.jpg</t>
   </si>
   <si>
@@ -189,9 +171,6 @@
     <t xml:space="preserve">Carpinus betulus</t>
   </si>
   <si>
-    <t xml:space="preserve">obicni_grab_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 25 m</t>
   </si>
   <si>
@@ -204,7 +183,7 @@
     <t xml:space="preserve">glatka, ispucana</t>
   </si>
   <si>
-    <t xml:space="preserve">obicni_grab_krosnja</t>
+    <t xml:space="preserve">obicni_grab_krosnja.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.plantea.com.hr/obicni-grab/</t>
@@ -216,9 +195,6 @@
     <t xml:space="preserve">Castanea sativa</t>
   </si>
   <si>
-    <t xml:space="preserve">pitomi_kesten_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">preko 30 m</t>
   </si>
   <si>
@@ -231,7 +207,7 @@
     <t xml:space="preserve">glatka, uzdužno ispucana</t>
   </si>
   <si>
-    <t xml:space="preserve">pitomi_kesten_krosnja</t>
+    <t xml:space="preserve">pitomi_kesten_krosnja.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.plantea.com.hr/pitomi-kesten/</t>
@@ -243,9 +219,6 @@
     <t xml:space="preserve">Acer campestre</t>
   </si>
   <si>
-    <t xml:space="preserve">klen_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">klen_plod.jpg</t>
   </si>
   <si>
@@ -255,7 +228,7 @@
     <t xml:space="preserve">glatka, mrežasto ispucana</t>
   </si>
   <si>
-    <t xml:space="preserve">klen_krosnja.jog</t>
+    <t xml:space="preserve">klen_krosnja.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.plantea.com.hr/javor-klen/</t>
@@ -267,9 +240,6 @@
     <t xml:space="preserve">Celtis australis</t>
   </si>
   <si>
-    <t xml:space="preserve">kostela_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">kostela_plod.jpg</t>
   </si>
   <si>
@@ -288,9 +258,6 @@
     <t xml:space="preserve">Alnus glutinosa</t>
   </si>
   <si>
-    <t xml:space="preserve">crna_joha_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">crna_joha_plod.jpg</t>
   </si>
   <si>
@@ -312,9 +279,6 @@
     <t xml:space="preserve">Betula pendula</t>
   </si>
   <si>
-    <t xml:space="preserve">obicna_breza_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 30 m</t>
   </si>
   <si>
@@ -339,9 +303,6 @@
     <t xml:space="preserve">Acer pseudo platanus</t>
   </si>
   <si>
-    <t xml:space="preserve">gorski_javor_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 40 m</t>
   </si>
   <si>
@@ -366,9 +327,6 @@
     <t xml:space="preserve">Ceratonia siliqua</t>
   </si>
   <si>
-    <t xml:space="preserve">rogac_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 15 m</t>
   </si>
   <si>
@@ -390,9 +348,6 @@
     <t xml:space="preserve">Crateagus monogyna</t>
   </si>
   <si>
-    <t xml:space="preserve">bijeli_glog_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 8 m</t>
   </si>
   <si>
@@ -417,10 +372,7 @@
     <t xml:space="preserve">Fagus sylvatica</t>
   </si>
   <si>
-    <t xml:space="preserve">obicna_bukva_list.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obicna_bukva_plod.jog</t>
+    <t xml:space="preserve">obicna_bukva_plod.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">maslinastozelena, pepeljastosiva</t>
@@ -438,9 +390,6 @@
     <t xml:space="preserve">Fraxinus angustifolia</t>
   </si>
   <si>
-    <t xml:space="preserve">poljski_jasen_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">poljski_jasen_plod.jpg</t>
   </si>
   <si>
@@ -462,9 +411,6 @@
     <t xml:space="preserve">Fraxinus excelsior</t>
   </si>
   <si>
-    <t xml:space="preserve">obicni_jasen_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">obicni_jasen_plod.jpg</t>
   </si>
   <si>
@@ -483,9 +429,6 @@
     <t xml:space="preserve">Fraxinus ornus</t>
   </si>
   <si>
-    <t xml:space="preserve">crni_jasen_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">crni_jasen_plod.jpg</t>
   </si>
   <si>
@@ -504,9 +447,6 @@
     <t xml:space="preserve">Ilex aquifolium</t>
   </si>
   <si>
-    <t xml:space="preserve">bozikovina_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 5 m</t>
   </si>
   <si>
@@ -519,7 +459,7 @@
     <t xml:space="preserve">glatka, raspucana</t>
   </si>
   <si>
-    <t xml:space="preserve">bozikovina_korsnja.jpeg</t>
+    <t xml:space="preserve">bozikovina_krosnja.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.plantea.com.hr/bozikovina/</t>
@@ -531,9 +471,6 @@
     <t xml:space="preserve">Juglans nigra</t>
   </si>
   <si>
-    <t xml:space="preserve">crni_orah_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">crni_orah_plod.jpg</t>
   </si>
   <si>
@@ -555,9 +492,6 @@
     <t xml:space="preserve">Juglans regia</t>
   </si>
   <si>
-    <t xml:space="preserve">obicni_orah_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">obicni_orah_plod.jpg</t>
   </si>
   <si>
@@ -579,9 +513,6 @@
     <t xml:space="preserve">Laurus nobilis</t>
   </si>
   <si>
-    <t xml:space="preserve">lovor_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 18 m</t>
   </si>
   <si>
@@ -600,9 +531,6 @@
     <t xml:space="preserve">Malus domestica</t>
   </si>
   <si>
-    <t xml:space="preserve">jabuka_list</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 12 m</t>
   </si>
   <si>
@@ -624,9 +552,6 @@
     <t xml:space="preserve">Olea europaea</t>
   </si>
   <si>
-    <t xml:space="preserve">divlja_maslina_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 10 m</t>
   </si>
   <si>
@@ -648,9 +573,6 @@
     <t xml:space="preserve">Ostrya carpinifolia</t>
   </si>
   <si>
-    <t xml:space="preserve">crni_grab_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">crni_grab_plod.jpg</t>
   </si>
   <si>
@@ -672,9 +594,6 @@
     <t xml:space="preserve">Populus alba</t>
   </si>
   <si>
-    <t xml:space="preserve">bijela_topola_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 35 m</t>
   </si>
   <si>
@@ -699,9 +618,6 @@
     <t xml:space="preserve">Populus canescens</t>
   </si>
   <si>
-    <t xml:space="preserve">siva_topola_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">siva_topola_plod.jpg</t>
   </si>
   <si>
@@ -720,9 +636,6 @@
     <t xml:space="preserve">Populus nigra</t>
   </si>
   <si>
-    <t xml:space="preserve">crna_topola_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">crna_topola_plod.jpg</t>
   </si>
   <si>
@@ -744,9 +657,6 @@
     <t xml:space="preserve">Prunus avium</t>
   </si>
   <si>
-    <t xml:space="preserve">divlja_tresnja_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">divlja_tresnja_plod.jpg</t>
   </si>
   <si>
@@ -768,9 +678,6 @@
     <t xml:space="preserve">Prunus dulcis</t>
   </si>
   <si>
-    <t xml:space="preserve">badem_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">badem_plod.jpg</t>
   </si>
   <si>
@@ -789,9 +696,6 @@
     <t xml:space="preserve">Pyrus communis</t>
   </si>
   <si>
-    <t xml:space="preserve">pitoma_kruska_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">pitoma_kruska_plod.jpg</t>
   </si>
   <si>
@@ -810,9 +714,6 @@
     <t xml:space="preserve">Quercus cerris</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_cer_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">hrast_cer_plod.jpg</t>
   </si>
   <si>
@@ -831,9 +732,6 @@
     <t xml:space="preserve">Quercus coccifera</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_ostrika_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">od 2 do 6 m</t>
   </si>
   <si>
@@ -855,9 +753,6 @@
     <t xml:space="preserve">Quercus frainetto</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_sladun_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">hrast_sladun_plod.jpg</t>
   </si>
   <si>
@@ -876,9 +771,6 @@
     <t xml:space="preserve">Quercus ilex</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_crnika_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">hrast_crnika_plod.jpg</t>
   </si>
   <si>
@@ -897,9 +789,6 @@
     <t xml:space="preserve">Quercus petraea</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_kitnjak_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">hrast_kitnjak_plod.jpg</t>
   </si>
   <si>
@@ -918,9 +807,6 @@
     <t xml:space="preserve">Quercus pubescens</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_medunac_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">do 20 m </t>
   </si>
   <si>
@@ -942,9 +828,6 @@
     <t xml:space="preserve">Quercus robur</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_luznjak_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">hrast_luznjak_plod.jpg</t>
   </si>
   <si>
@@ -966,9 +849,6 @@
     <t xml:space="preserve">Quercus rubra	</t>
   </si>
   <si>
-    <t xml:space="preserve">cerveni_hrast_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">cerveni_hrast_plod.jpg</t>
   </si>
   <si>
@@ -987,9 +867,6 @@
     <t xml:space="preserve">Quercus suber</t>
   </si>
   <si>
-    <t xml:space="preserve">hrast_plutnjak_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">hrast_plutnjak_plod.jpg</t>
   </si>
   <si>
@@ -1008,9 +885,6 @@
     <t xml:space="preserve">Robinia pseudoacacia</t>
   </si>
   <si>
-    <t xml:space="preserve">obicni_bagrem_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">obicni_bagrem_plod.jpg</t>
   </si>
   <si>
@@ -1029,9 +903,6 @@
     <t xml:space="preserve">Salix alba</t>
   </si>
   <si>
-    <t xml:space="preserve">bijela_vrba_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">bijela_vrba_plod.jpg</t>
   </si>
   <si>
@@ -1053,9 +924,6 @@
     <t xml:space="preserve">Salix caprea</t>
   </si>
   <si>
-    <t xml:space="preserve">vrba_iva_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">vrba_iva_plod.jpg</t>
   </si>
   <si>
@@ -1074,9 +942,6 @@
     <t xml:space="preserve">Salix cinerea</t>
   </si>
   <si>
-    <t xml:space="preserve">siva_vrba_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">4 do 15 m</t>
   </si>
   <si>
@@ -1098,9 +963,6 @@
     <t xml:space="preserve">Tilia cordata</t>
   </si>
   <si>
-    <t xml:space="preserve">malolisna_lipa_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">malolisna_lipa_plod.jpg</t>
   </si>
   <si>
@@ -1116,9 +978,6 @@
     <t xml:space="preserve">Tilia platyphyllos</t>
   </si>
   <si>
-    <t xml:space="preserve">velelisna_lipa_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">velelisna_lipa_plod.jpg</t>
   </si>
   <si>
@@ -1134,9 +993,6 @@
     <t xml:space="preserve">Ulmus glabra </t>
   </si>
   <si>
-    <t xml:space="preserve">gorski_brijest_list.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">gorski_brijest_plod.jpg</t>
   </si>
   <si>
@@ -1153,9 +1009,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ulmus minor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">poljski_brijest_list.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">poljski_brijest_plod.jpg</t>
@@ -1266,7 +1119,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1284,10 +1137,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1313,28 +1162,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="1:49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C2:C49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0445344129555"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.5425101214575"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7773279352227"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.3643724696356"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.3036437246964"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.2550607287449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.4453441295547"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.0121457489879"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.70445344129555"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1214574898785"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2550607287449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9352226720648"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4453441295547"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6113360323887"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.5991902834008"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.080971659919"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1362,1549 +1209,1414 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>57</v>
+        <v>50</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>68</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>82</v>
+        <v>72</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>89</v>
+        <v>78</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>81</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>98</v>
+        <v>86</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>107</v>
+        <v>94</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>97</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>153</v>
+        <v>11</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>154</v>
+        <v>51</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>177</v>
+        <v>85</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>194</v>
+        <v>29</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>203</v>
+        <v>103</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>208</v>
+        <v>49</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>56</v>
+        <v>183</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>225</v>
+        <v>85</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>97</v>
+        <v>198</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>232</v>
+        <v>85</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>97</v>
+        <v>204</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>240</v>
+        <v>85</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>247</v>
+        <v>217</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>248</v>
+        <v>176</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>250</v>
+        <v>185</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>254</v>
+      <c r="A32" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>255</v>
+        <v>169</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>256</v>
+        <v>13</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>15</v>
+        <v>225</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>262</v>
+        <v>93</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>106</v>
+        <v>230</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>263</v>
+        <v>73</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>83</v>
+        <v>231</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>264</v>
+        <v>232</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>268</v>
+        <v>235</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>270</v>
+      <c r="D34" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>271</v>
+        <v>13</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>15</v>
+        <v>238</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>272</v>
+        <v>239</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>277</v>
+        <v>49</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>56</v>
+        <v>243</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>278</v>
+        <v>51</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>58</v>
+        <v>244</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>284</v>
+        <v>11</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>285</v>
+        <v>157</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>179</v>
+        <v>250</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>291</v>
+        <v>93</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>106</v>
+        <v>255</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>292</v>
+        <v>13</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>15</v>
+        <v>256</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>295</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>299</v>
+        <v>262</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>300</v>
+        <v>29</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>33</v>
+        <v>263</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>301</v>
+        <v>264</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>303</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="AMJ38" s="0"/>
     </row>
     <row r="39" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>306</v>
+        <v>93</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>106</v>
+        <v>268</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>311</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="AMJ39" s="0"/>
     </row>
     <row r="40" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>314</v>
+        <v>85</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>97</v>
+        <v>275</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>315</v>
+        <v>73</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>83</v>
+        <v>276</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>316</v>
+        <v>277</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>318</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="AMJ40" s="0"/>
     </row>
     <row r="41" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>321</v>
+        <v>101</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>115</v>
+        <v>281</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>322</v>
+        <v>212</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>323</v>
+        <v>283</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>325</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="AMJ41" s="0"/>
     </row>
     <row r="42" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>326</v>
+        <v>285</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>327</v>
+        <v>286</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>328</v>
+        <v>49</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>56</v>
+        <v>287</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>329</v>
+        <v>212</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>330</v>
+        <v>289</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>332</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="AMJ42" s="0"/>
     </row>
     <row r="43" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>335</v>
+        <v>11</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>13</v>
+        <v>293</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>336</v>
+        <v>294</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>337</v>
+        <v>295</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>338</v>
+        <v>296</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>340</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="AMJ43" s="0"/>
     </row>
     <row r="44" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>341</v>
+        <v>298</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>342</v>
+        <v>299</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>343</v>
+        <v>169</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>193</v>
+        <v>300</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>344</v>
+        <v>130</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>148</v>
+        <v>301</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>345</v>
+        <v>302</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>347</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="AMJ44" s="0"/>
     </row>
     <row r="45" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>348</v>
+        <v>304</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>349</v>
+        <v>305</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>350</v>
+        <v>306</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>351</v>
+        <v>307</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>352</v>
+        <v>212</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>242</v>
+        <v>308</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>353</v>
+        <v>309</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>355</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="AMJ45" s="0"/>
     </row>
     <row r="46" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>356</v>
+        <v>311</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>357</v>
+        <v>312</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>358</v>
+        <v>49</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>56</v>
+        <v>313</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>359</v>
+        <v>212</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>242</v>
+        <v>158</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>180</v>
+        <v>314</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>361</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="AMJ46" s="0"/>
     </row>
     <row r="47" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>362</v>
+        <v>316</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>363</v>
+        <v>317</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>364</v>
+        <v>85</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>97</v>
+        <v>318</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>365</v>
+        <v>212</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>367</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="AMJ47" s="0"/>
     </row>
     <row r="48" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>368</v>
+        <v>321</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>369</v>
+        <v>322</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>370</v>
+        <v>93</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>106</v>
+        <v>323</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>371</v>
+        <v>29</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>33</v>
+        <v>324</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>372</v>
+        <v>325</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>374</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="AMJ48" s="0"/>
     </row>
     <row r="49" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>375</v>
+        <v>327</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>376</v>
+        <v>328</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>377</v>
+        <v>93</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>106</v>
+        <v>329</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>378</v>
+        <v>330</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>379</v>
+        <v>331</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>380</v>
+        <v>332</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>382</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="AMJ49" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="https://www.plantea.com.hr/makedonski-hrast/"/>
+    <hyperlink ref="I2" r:id="rId1" display="https://www.plantea.com.hr/makedonski-hrast/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2924,13 +2636,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C49 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70445344129555"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2950,13 +2659,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C49 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70445344129555"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>